<commit_message>
Revert "My 25 added"
This reverts commit f3dd0b90de040dab16ea2436d242a08bc94d21de.
</commit_message>
<xml_diff>
--- a/Patient details.xlsx
+++ b/Patient details.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor_000\Documents\a.SD\GitHub\Software-Testing-And-Verification\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="456">
   <si>
     <t>NHS Number</t>
   </si>
@@ -1387,147 +1382,6 @@
   </si>
   <si>
     <t>Gluten</t>
-  </si>
-  <si>
-    <t>Chloe</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Carol</t>
-  </si>
-  <si>
-    <t>Fiona</t>
-  </si>
-  <si>
-    <t>Grace</t>
-  </si>
-  <si>
-    <t>Hannah</t>
-  </si>
-  <si>
-    <t>Ava</t>
-  </si>
-  <si>
-    <t>Michelle</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Emma</t>
-  </si>
-  <si>
-    <t>Rachel</t>
-  </si>
-  <si>
-    <t>Rose</t>
-  </si>
-  <si>
-    <t>Nicola</t>
-  </si>
-  <si>
-    <t>Alan</t>
-  </si>
-  <si>
-    <t>Colin</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Ruth</t>
-  </si>
-  <si>
-    <t>Connor</t>
-  </si>
-  <si>
-    <t>Jake</t>
-  </si>
-  <si>
-    <t>Frank</t>
-  </si>
-  <si>
-    <t>Gavin</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>Richard</t>
-  </si>
-  <si>
-    <t>Sean</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Davies</t>
-  </si>
-  <si>
-    <t>Fisher</t>
-  </si>
-  <si>
-    <t>Nolan</t>
-  </si>
-  <si>
-    <t>Morgan</t>
-  </si>
-  <si>
-    <t>Peake</t>
-  </si>
-  <si>
-    <t>McDonald</t>
-  </si>
-  <si>
-    <t>Quinn</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>Underwood</t>
-  </si>
-  <si>
-    <t>Vaughan</t>
-  </si>
-  <si>
-    <t>Hart</t>
-  </si>
-  <si>
-    <t>Cameron</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>Coleman</t>
-  </si>
-  <si>
-    <t>Knox</t>
-  </si>
-  <si>
-    <t>King</t>
-  </si>
-  <si>
-    <t>Lewis</t>
-  </si>
-  <si>
-    <t>Moore</t>
-  </si>
-  <si>
-    <t>Kelly</t>
-  </si>
-  <si>
-    <t>Mackay</t>
-  </si>
-  <si>
-    <t>Morrison</t>
-  </si>
-  <si>
-    <t>Mills</t>
   </si>
 </sst>
 </file>
@@ -1577,9 +1431,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1627,7 +1478,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1662,7 +1513,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1873,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,12 +2222,6 @@
       <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>481</v>
-      </c>
       <c r="E21" t="s">
         <v>381</v>
       </c>
@@ -2395,12 +2240,6 @@
       <c r="B22" t="s">
         <v>8</v>
       </c>
-      <c r="C22" t="s">
-        <v>480</v>
-      </c>
-      <c r="D22" t="s">
-        <v>482</v>
-      </c>
       <c r="E22" t="s">
         <v>401</v>
       </c>
@@ -2419,12 +2258,6 @@
       <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="C23" t="s">
-        <v>456</v>
-      </c>
-      <c r="D23" t="s">
-        <v>457</v>
-      </c>
       <c r="E23" t="s">
         <v>442</v>
       </c>
@@ -2442,12 +2275,6 @@
       <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
-        <v>479</v>
-      </c>
-      <c r="D24" t="s">
-        <v>483</v>
-      </c>
       <c r="E24" t="s">
         <v>323</v>
       </c>
@@ -2465,12 +2292,6 @@
       <c r="B25" t="s">
         <v>8</v>
       </c>
-      <c r="C25" t="s">
-        <v>478</v>
-      </c>
-      <c r="D25" t="s">
-        <v>484</v>
-      </c>
       <c r="E25" t="s">
         <v>329</v>
       </c>
@@ -2488,12 +2309,6 @@
       <c r="B26" t="s">
         <v>9</v>
       </c>
-      <c r="C26" t="s">
-        <v>458</v>
-      </c>
-      <c r="D26" t="s">
-        <v>485</v>
-      </c>
       <c r="E26" t="s">
         <v>321</v>
       </c>
@@ -2511,12 +2326,6 @@
       <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="C27" t="s">
-        <v>459</v>
-      </c>
-      <c r="D27" t="s">
-        <v>486</v>
-      </c>
       <c r="E27" t="s">
         <v>299</v>
       </c>
@@ -2534,12 +2343,6 @@
       <c r="B28" t="s">
         <v>8</v>
       </c>
-      <c r="C28" t="s">
-        <v>477</v>
-      </c>
-      <c r="D28" t="s">
-        <v>487</v>
-      </c>
       <c r="E28" t="s">
         <v>435</v>
       </c>
@@ -2557,12 +2360,6 @@
       <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="C29" t="s">
-        <v>468</v>
-      </c>
-      <c r="D29" t="s">
-        <v>488</v>
-      </c>
       <c r="E29" t="s">
         <v>409</v>
       </c>
@@ -2580,12 +2377,6 @@
       <c r="B30" t="s">
         <v>8</v>
       </c>
-      <c r="C30" t="s">
-        <v>475</v>
-      </c>
-      <c r="D30" t="s">
-        <v>489</v>
-      </c>
       <c r="E30" t="s">
         <v>414</v>
       </c>
@@ -2603,12 +2394,6 @@
       <c r="B31" t="s">
         <v>8</v>
       </c>
-      <c r="C31" t="s">
-        <v>476</v>
-      </c>
-      <c r="D31" t="s">
-        <v>490</v>
-      </c>
       <c r="E31" t="s">
         <v>384</v>
       </c>
@@ -2626,12 +2411,6 @@
       <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="C32" t="s">
-        <v>467</v>
-      </c>
-      <c r="D32" t="s">
-        <v>491</v>
-      </c>
       <c r="E32" t="s">
         <v>404</v>
       </c>
@@ -2649,12 +2428,6 @@
       <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="C33" t="s">
-        <v>474</v>
-      </c>
-      <c r="D33" t="s">
-        <v>492</v>
-      </c>
       <c r="E33" t="s">
         <v>420</v>
       </c>
@@ -2673,12 +2446,6 @@
       <c r="B34" t="s">
         <v>8</v>
       </c>
-      <c r="C34" t="s">
-        <v>473</v>
-      </c>
-      <c r="D34" t="s">
-        <v>493</v>
-      </c>
       <c r="E34" t="s">
         <v>332</v>
       </c>
@@ -2696,12 +2463,6 @@
       <c r="B35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" t="s">
-        <v>466</v>
-      </c>
-      <c r="D35" t="s">
-        <v>494</v>
-      </c>
       <c r="E35" t="s">
         <v>407</v>
       </c>
@@ -2719,12 +2480,6 @@
       <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C36" t="s">
-        <v>465</v>
-      </c>
-      <c r="D36" t="s">
-        <v>495</v>
-      </c>
       <c r="E36" t="s">
         <v>405</v>
       </c>
@@ -2742,12 +2497,6 @@
       <c r="B37" t="s">
         <v>9</v>
       </c>
-      <c r="C37" t="s">
-        <v>464</v>
-      </c>
-      <c r="D37" t="s">
-        <v>496</v>
-      </c>
       <c r="E37" t="s">
         <v>68</v>
       </c>
@@ -2765,12 +2514,6 @@
       <c r="B38" t="s">
         <v>9</v>
       </c>
-      <c r="C38" t="s">
-        <v>463</v>
-      </c>
-      <c r="D38" t="s">
-        <v>497</v>
-      </c>
       <c r="E38" t="s">
         <v>373</v>
       </c>
@@ -2789,12 +2532,6 @@
       <c r="B39" t="s">
         <v>9</v>
       </c>
-      <c r="C39" t="s">
-        <v>462</v>
-      </c>
-      <c r="D39" t="s">
-        <v>498</v>
-      </c>
       <c r="E39" t="s">
         <v>379</v>
       </c>
@@ -2812,12 +2549,6 @@
       <c r="B40" t="s">
         <v>10</v>
       </c>
-      <c r="C40" t="s">
-        <v>461</v>
-      </c>
-      <c r="D40" t="s">
-        <v>499</v>
-      </c>
       <c r="E40" t="s">
         <v>289</v>
       </c>
@@ -2836,12 +2567,6 @@
       <c r="B41" t="s">
         <v>11</v>
       </c>
-      <c r="C41" t="s">
-        <v>472</v>
-      </c>
-      <c r="D41" t="s">
-        <v>500</v>
-      </c>
       <c r="E41" t="s">
         <v>427</v>
       </c>
@@ -2859,12 +2584,6 @@
       <c r="B42" t="s">
         <v>10</v>
       </c>
-      <c r="C42" t="s">
-        <v>460</v>
-      </c>
-      <c r="D42" t="s">
-        <v>497</v>
-      </c>
       <c r="E42" t="s">
         <v>290</v>
       </c>
@@ -2883,12 +2602,6 @@
       <c r="B43" t="s">
         <v>8</v>
       </c>
-      <c r="C43" t="s">
-        <v>471</v>
-      </c>
-      <c r="D43" t="s">
-        <v>483</v>
-      </c>
       <c r="E43" t="s">
         <v>302</v>
       </c>
@@ -2907,12 +2620,6 @@
       <c r="B44" t="s">
         <v>8</v>
       </c>
-      <c r="C44" t="s">
-        <v>470</v>
-      </c>
-      <c r="D44" t="s">
-        <v>502</v>
-      </c>
       <c r="E44" t="s">
         <v>301</v>
       </c>
@@ -2929,12 +2636,6 @@
       </c>
       <c r="B45" t="s">
         <v>8</v>
-      </c>
-      <c r="C45" t="s">
-        <v>469</v>
-      </c>
-      <c r="D45" t="s">
-        <v>501</v>
       </c>
       <c r="E45" t="s">
         <v>293</v>

</xml_diff>